<commit_message>
Updated files for better readability
</commit_message>
<xml_diff>
--- a/Spporting_info_and_db/Areas_Estados.xlsx
+++ b/Spporting_info_and_db/Areas_Estados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Documents\IronHack\data-visualization-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Documents\_IronHack\data-visualization-project\Spporting_info_and_db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A488214-1B6B-436B-BA62-6E4B486F3728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF372BB7-04E3-4FC4-842B-209BD1D51A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="8535" windowWidth="20730" windowHeight="11160" xr2:uid="{DEA101CB-24B7-4BFF-A81B-101581E990F2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Chihuahua</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Superficie km2</t>
+  </si>
+  <si>
+    <t>Superficie_m2</t>
   </si>
 </sst>
 </file>
@@ -487,278 +490,412 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAEDDA4-086E-4E8F-9304-14A7A492FCD1}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2">
         <v>5616</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <f>B2*1000*1000</f>
+        <v>5616000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3">
         <v>71450</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <f t="shared" ref="C3:C33" si="0">B3*1000*1000</f>
+        <v>71450000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4">
         <v>73909</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>73909000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5">
         <v>57507</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>57507000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6">
         <v>73311</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>73311000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
       <c r="B7">
         <v>247455</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>247455000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>31</v>
       </c>
       <c r="B8">
         <v>1495</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>1495000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9">
         <v>151562</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>151562000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
       <c r="B10">
         <v>5627</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>5627000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11">
         <v>123317</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>123317000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
       <c r="B12">
         <v>22351</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>22351000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
       <c r="B13">
         <v>30608</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>30608000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
         <v>63596</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>63596000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
       <c r="B15">
         <v>20813</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>20813000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16">
         <v>78588</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>78588000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17">
         <v>58599</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>58599000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
       <c r="B18">
         <v>4879</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>4879000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
       <c r="B19">
         <v>27857</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>27857000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
       <c r="B20">
         <v>64156</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>64156000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>
       <c r="B21">
         <v>93757</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>93757000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22">
         <v>34306</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>34306000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
       <c r="B23">
         <v>11699</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>11699000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
       <c r="B24">
         <v>44705</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>44705000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>14</v>
       </c>
       <c r="B25">
         <v>61137</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>61137000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
       <c r="B26">
         <v>58200</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>58200000000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1</v>
       </c>
       <c r="B27">
         <v>179355</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>179355000000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>23</v>
       </c>
       <c r="B28">
         <v>24731</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>24731000000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
       <c r="B29">
         <v>80249</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>80249000000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30">
         <v>4016</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>4016000000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>10</v>
       </c>
       <c r="B31">
         <v>71826</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>71826000000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>19</v>
       </c>
       <c r="B32">
         <v>39524</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>39524000000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>7</v>
       </c>
       <c r="B33">
         <v>75284</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>75284000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>